<commit_message>
A few bug fixes for modules to run in unit test mode Producer module now uses GHGStandard to calculate Mg     Vehicles can have different footprints and it gets handled properly Producer module now correctly calculates target Mg for each factorial combination     Winning combo is one that generates credits (complies or over complies) at the lowest cost Minor change to batch file format (so KBo won't be as confused)
</commit_message>
<xml_diff>
--- a/inputs/phase0_default_batch_file.xlsx
+++ b/inputs/phase0_default_batch_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CEEB0B-AD7A-4C98-821D-B315C30DC12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BF32D5-940C-4CD1-AB7B-7B47FC8B4FAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="150" windowWidth="23415" windowHeight="19650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1185" yWindow="1635" windowWidth="27360" windowHeight="17250" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>String</t>
   </si>
   <si>
-    <t>Session Output Path</t>
-  </si>
-  <si>
     <t>Batch Name</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>#</t>
-  </si>
-  <si>
-    <t>Database Dump Path</t>
   </si>
   <si>
     <t>Manufacturers File</t>
@@ -205,6 +199,12 @@
   </si>
   <si>
     <t>CostCurves</t>
+  </si>
+  <si>
+    <t>Session Output Folder Name</t>
+  </si>
+  <si>
+    <t>Database Dump Folder Name</t>
   </si>
 </sst>
 </file>
@@ -701,7 +701,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
@@ -759,7 +759,7 @@
     </row>
     <row r="2" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -779,13 +779,13 @@
     </row>
     <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -822,7 +822,7 @@
     </row>
     <row r="5" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
@@ -842,10 +842,10 @@
     </row>
     <row r="6" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="8" t="b">
         <v>1</v>
@@ -877,10 +877,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -900,16 +900,16 @@
     </row>
     <row r="8" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -949,7 +949,7 @@
     </row>
     <row r="10" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -971,16 +971,16 @@
     </row>
     <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1000,16 +1000,16 @@
     </row>
     <row r="12" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1029,16 +1029,16 @@
     </row>
     <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1058,16 +1058,16 @@
     </row>
     <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1087,16 +1087,16 @@
     </row>
     <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1116,16 +1116,16 @@
     </row>
     <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1145,16 +1145,16 @@
     </row>
     <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1174,16 +1174,16 @@
     </row>
     <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1203,16 +1203,16 @@
     </row>
     <row r="19" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1232,16 +1232,16 @@
     </row>
     <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1261,16 +1261,16 @@
     </row>
     <row r="21" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1290,16 +1290,16 @@
     </row>
     <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1319,10 +1319,10 @@
     </row>
     <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23" s="10" t="b">
         <v>1</v>
@@ -1348,10 +1348,10 @@
     </row>
     <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="8" t="b">
         <v>1</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="27" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -1436,16 +1436,16 @@
     </row>
     <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -1465,16 +1465,16 @@
     </row>
     <row r="29" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" s="8">
         <v>0.75</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="33" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
@@ -1586,16 +1586,16 @@
     </row>
     <row r="34" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1615,16 +1615,16 @@
     </row>
     <row r="35" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>

</xml_diff>

<commit_message>
fix to default batch for gcam file rename refinements to batch process     bundled expanded batch files now use relative paths for inputs so they should be more portable     bundled expanded batch shows where it came from originally
</commit_message>
<xml_diff>
--- a/inputs/phase0_default_batch_file.xlsx
+++ b/inputs/phase0_default_batch_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BF32D5-940C-4CD1-AB7B-7B47FC8B4FAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E022DABC-8C7D-409A-8587-464204F4BFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="1635" windowWidth="27360" windowHeight="17250" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9195" yWindow="165" windowWidth="13410" windowHeight="16305" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>input_templates/vehicles.csv</t>
   </si>
   <si>
-    <t>input_templates/demanded_sales_annual_data.csv</t>
-  </si>
-  <si>
     <t>input_templates/fuel_scenarios.csv</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>Database Dump Folder Name</t>
+  </si>
+  <si>
+    <t>input_templates/demanded_shares-gcam.csv</t>
   </si>
 </sst>
 </file>
@@ -699,9 +699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +785,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -877,10 +877,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -900,7 +900,7 @@
     </row>
     <row r="8" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
@@ -1093,10 +1093,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1151,10 +1151,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1180,10 +1180,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1206,13 +1206,13 @@
         <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1238,10 +1238,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1267,10 +1267,10 @@
         <v>26</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1296,10 +1296,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>13</v>
@@ -1445,7 +1445,7 @@
         <v>10</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>13</v>
@@ -1592,10 +1592,10 @@
         <v>27</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1621,10 +1621,10 @@
         <v>27</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>

</xml_diff>

<commit_message>
more gcam changes to fix KBo bug
</commit_message>
<xml_diff>
--- a/inputs/phase0_default_batch_file.xlsx
+++ b/inputs/phase0_default_batch_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E022DABC-8C7D-409A-8587-464204F4BFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7336C611-6EA2-4204-9B6F-370923FD510F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9195" yWindow="165" windowWidth="13410" windowHeight="16305" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="885" windowWidth="19305" windowHeight="16305" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>Vehicles File</t>
   </si>
   <si>
-    <t>Demanded Annual Sales File</t>
-  </si>
-  <si>
     <t>Fuel Scenarios File</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>input_templates/demanded_shares-gcam.csv</t>
+  </si>
+  <si>
+    <t>Demanded Shares File</t>
   </si>
 </sst>
 </file>
@@ -699,9 +699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,7 +785,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -877,10 +877,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -900,16 +900,16 @@
     </row>
     <row r="8" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -971,16 +971,16 @@
     </row>
     <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1006,10 +1006,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1035,10 +1035,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1064,10 +1064,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1087,16 +1087,16 @@
     </row>
     <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1116,16 +1116,16 @@
     </row>
     <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1145,16 +1145,16 @@
     </row>
     <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1174,16 +1174,16 @@
     </row>
     <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1203,16 +1203,16 @@
     </row>
     <row r="19" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1232,16 +1232,16 @@
     </row>
     <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1261,16 +1261,16 @@
     </row>
     <row r="21" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="C21" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1290,16 +1290,16 @@
     </row>
     <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1348,7 +1348,7 @@
     </row>
     <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>13</v>
@@ -1445,7 +1445,7 @@
         <v>10</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="29" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>11</v>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>13</v>
@@ -1586,16 +1586,16 @@
     </row>
     <row r="34" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1615,16 +1615,16 @@
     </row>
     <row r="35" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>

</xml_diff>

<commit_message>
just a little dispy cleanup default batch turns off VERBOSE (otherwise generates insane amounts of console output during batch processing!)
</commit_message>
<xml_diff>
--- a/inputs/phase0_default_batch_file.xlsx
+++ b/inputs/phase0_default_batch_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7336C611-6EA2-4204-9B6F-370923FD510F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F698BE4-844E-4375-A449-5B96738722A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="885" windowWidth="19305" windowHeight="16305" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3975" yWindow="945" windowWidth="29445" windowHeight="18255" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -700,8 +700,8 @@
   <dimension ref="A1:AG36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="7" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,10 +1325,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>

</xml_diff>